<commit_message>
W01 Winter 2021 Prep.
</commit_message>
<xml_diff>
--- a/Assistants/Schedule_Duties_Info.xlsx
+++ b/Assistants/Schedule_Duties_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hosseinfani/Google_Drive/Academic/UWindsor/Course/COMP2650/Semester/W2021_Hossein Fani/Assistants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfani\Google_Drive\Academic\UWindsor\Course\COMP2650_Digital_Design\W2021_Hossein_Fani\Assistants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A4BC04-866F-354E-A32C-055920593BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F5D968-AFFF-4CDA-9239-009D97189D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="2" xr2:uid="{2C32AA88-CB60-44B0-A959-D17D6FFE0192}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C32AA88-CB60-44B0-A959-D17D6FFE0192}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Marking
 - 7:00</t>
@@ -55,20 +55,10 @@
 7:00 - </t>
   </si>
   <si>
-    <t>Lab Sections 51 &amp; 55
-19:00-22:00</t>
-  </si>
-  <si>
-    <t>GA2</t>
-  </si>
-  <si>
     <t>Lab Sections 53 &amp; 52
 16:00-19:00</t>
   </si>
   <si>
-    <t>GA1</t>
-  </si>
-  <si>
     <t>Moderate Lecture &amp; Office B
 10:00-12:30</t>
   </si>
@@ -158,9 +148,6 @@
     <t>Khalid</t>
   </si>
   <si>
-    <t>Muhammad</t>
-  </si>
-  <si>
     <t>Hours Allocated </t>
   </si>
   <si>
@@ -182,9 +169,6 @@
     <t>Marker</t>
   </si>
   <si>
-    <t>GA1-2</t>
-  </si>
-  <si>
     <t>Lab Instructor</t>
   </si>
   <si>
@@ -210,9 +194,6 @@
   </si>
   <si>
     <t>patel891</t>
-  </si>
-  <si>
-    <t>TA2</t>
   </si>
   <si>
     <t>Monitor Discussion Board</t>
@@ -626,19 +607,10 @@
     </r>
   </si>
   <si>
-    <t>TA3: Faraz
-TA4: Misha
-TA5: Dhwani</t>
-  </si>
-  <si>
     <t xml:space="preserve">    TA1: Ariya</t>
   </si>
   <si>
     <t>TA1: Ariya</t>
-  </si>
-  <si>
-    <t>TA3: Faraz
-TA4: Misha  TA5: Dhwani</t>
   </si>
   <si>
     <t>Hi, Im Moeed. Currently doing my MSc Computer Science with my research being in cancer detection using Siamese neural networks. I have worked before as a data analyst, a software engineer, a full stack web developer as well as an associate AI engineer. This is my second term at uWindsor and my second term as a GA. Looking forward to working as  a GA in this course.</t>
@@ -658,6 +630,34 @@
   </si>
   <si>
     <t>Hello, I am Misha, currently in my third year of Computer Science. I have been TA for a year now and I am very much glad to a be TA in this course</t>
+  </si>
+  <si>
+    <t>Lab Sections 51 &amp; 54
+19:00-22:00</t>
+  </si>
+  <si>
+    <t>GA2: Manil</t>
+  </si>
+  <si>
+    <t>TA2: Misha</t>
+  </si>
+  <si>
+    <t>TA3: Faraz
+TA4: Ravi
+TA5: Dhwani</t>
+  </si>
+  <si>
+    <t>Muhammad Moeed</t>
+  </si>
+  <si>
+    <t>GA1: Moeed
+GA2: Manil</t>
+  </si>
+  <si>
+    <t>GA1: Moeed</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1076,9 +1076,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1129,6 +1126,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1411,7 +1414,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1100384</xdr:colOff>
+      <xdr:colOff>1014659</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>1257300</xdr:rowOff>
     </xdr:to>
@@ -1776,71 +1779,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22DDC83-E6A0-4CCE-B325-D7BC8822C4D5}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="20.33203125" style="1"/>
+    <col min="1" max="1" width="19.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="20.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>13</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="F1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>72</v>
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="18"/>
       <c r="D2" s="23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -1848,15 +1851,15 @@
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
     </row>
-    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
-        <v>5</v>
+    <row r="3" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -1865,15 +1868,15 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>3</v>
+    <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -1882,35 +1885,35 @@
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>53</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>74</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="C5" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
       <c r="B6" s="19"/>
       <c r="C6" s="18"/>
       <c r="D6" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="19"/>
@@ -1918,26 +1921,26 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
-        <v>70</v>
+    <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J8" s="2"/>
     </row>
   </sheetData>
@@ -1956,71 +1959,71 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="230.33203125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="1" width="20.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="230.28515625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="128" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="160" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="196.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
-        <v>43</v>
+    <row r="5" spans="1:4" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2032,236 +2035,239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90F77D-24DA-4093-923B-91E32C079022}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.5" style="29" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="29"/>
+    <col min="1" max="1" width="15.28515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.42578125" style="28" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="46" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="45"/>
+      <c r="D1" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="29">
+        <v>110036981</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="29">
+        <v>140</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="29">
+        <v>110023689</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="29">
+        <v>140</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="29">
+        <v>105127455</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="29">
+        <v>100</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="29">
+        <v>105140023</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="29">
+        <v>100</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="29">
+        <v>105175694</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="F6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="29">
+        <v>100</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="30">
-        <v>110036981</v>
-      </c>
-      <c r="E2" s="30" t="s">
+    <row r="7" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="29">
+        <v>110009274</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="30">
-        <v>140</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>74</v>
+      <c r="F7" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="29">
+        <v>100</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="30">
-        <v>110023689</v>
-      </c>
-      <c r="E3" s="30" t="s">
+    <row r="8" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="29">
+        <v>110028937</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="30">
-        <v>140</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="30">
-        <v>105127455</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="30">
+      <c r="F8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="29">
         <v>100</v>
       </c>
-      <c r="I4" s="40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="30">
-        <v>105140023</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="30">
-        <v>100</v>
-      </c>
-      <c r="I5" s="40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="30">
-        <v>105175694</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="30">
-        <v>100</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="30">
-        <v>110009274</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="30">
-        <v>100</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="30">
-        <v>110028937</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="30">
-        <v>100</v>
-      </c>
-      <c r="I8" s="41" t="s">
-        <v>77</v>
+      <c r="I8" s="40" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>